<commit_message>
somatic and align file outputs
</commit_message>
<xml_diff>
--- a/template_examples/wes_combined_analysis_template.xlsx
+++ b/template_examples/wes_combined_analysis_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E831B3-4863-FE42-896B-847E2396FCED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8F4DF4-705B-7941-9D5E-55B5611BBA1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WES Analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="WES Combined Analysis" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -60,7 +60,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+          <t>Path to a file on a user's computer.</t>
         </r>
       </text>
     </comment>
@@ -95,20 +95,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a user's computer.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -121,12 +108,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="17">
   <si>
     <t>#t</t>
   </si>
   <si>
-    <t>Wes analysis template</t>
+    <t>Wes combined analysis template</t>
   </si>
   <si>
     <t>#p</t>
@@ -147,13 +134,10 @@
     <t>#d</t>
   </si>
   <si>
-    <t>Cimac id</t>
+    <t>Tumor cimac id</t>
   </si>
   <si>
-    <t>Tumor</t>
-  </si>
-  <si>
-    <t>Normal</t>
+    <t>Normal cimac id</t>
   </si>
   <si>
     <t>Somatic</t>
@@ -171,23 +155,17 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>tumor</t>
-  </si>
-  <si>
-    <t>normal</t>
+    <t>germline</t>
   </si>
   <si>
     <t>somatic</t>
-  </si>
-  <si>
-    <t>germline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +184,18 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -274,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -285,6 +275,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,7 +617,7 @@
   <dimension ref="A1:F206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -635,7 +626,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -655,7 +646,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -669,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -682,7 +673,6 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -700,28 +690,22 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1722,7 +1706,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>